<commit_message>
Adicionando a daily 30/09, atualização no arquivo de entregaveisSprint2 e documentação
</commit_message>
<xml_diff>
--- a/reuniões/Organização Equipe/Entregáveis_Sprint2.xlsx
+++ b/reuniões/Organização Equipe/Entregáveis_Sprint2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/234fac80f67bd5e9/Área de Trabalho/SPTECH/projeto_sprint2/Documentacao/reuniões/Organização Equipe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\OrchisSystems\Documentacao\reuniões\Organização Equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{110DEF74-2206-4B74-9843-DF1037194BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02FA8C73-2B90-46F7-8DBF-479B63708F29}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976EB3D9-D4AD-4393-BD0B-9BF77099B26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2412B9C1-AE0B-4B06-99AA-23008C715C69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="45">
   <si>
     <t>Matéria</t>
   </si>
@@ -152,10 +152,25 @@
     <t>Fábio/Vinicius</t>
   </si>
   <si>
-    <t>Neto/Vinicius/Macari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fábio </t>
+    <t>Neto</t>
+  </si>
+  <si>
+    <t>Vinicius</t>
+  </si>
+  <si>
+    <t>Fabio(PO)</t>
+  </si>
+  <si>
+    <t>Responsável Semanal</t>
+  </si>
+  <si>
+    <t>Responsável Pai</t>
+  </si>
+  <si>
+    <t>Vinicius/Neto</t>
+  </si>
+  <si>
+    <t>Thais(SM)</t>
   </si>
 </sst>
 </file>
@@ -505,10 +520,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -828,18 +839,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76284797-5698-42CC-AC6E-5DE53A4B9F1B}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57:C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="81.6640625" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -982,24 +993,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="19"/>
       <c r="B17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="21"/>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:4" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -1007,10 +1019,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A21" s="11" t="s">
         <v>3</v>
       </c>
@@ -1018,24 +1033,29 @@
         <v>4</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A22" s="11"/>
       <c r="B22" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A23" s="11"/>
       <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A24" s="12" t="s">
         <v>7</v>
       </c>
@@ -1043,24 +1063,29 @@
         <v>8</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+        <v>40</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A25" s="12"/>
       <c r="B25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A26" s="12"/>
       <c r="B26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="18"/>
-    </row>
-    <row r="27" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A27" s="11" t="s">
         <v>11</v>
       </c>
@@ -1068,56 +1093,71 @@
         <v>12</v>
       </c>
       <c r="C27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A28" s="11"/>
       <c r="B28" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="14"/>
-    </row>
-    <row r="29" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A29" s="11"/>
       <c r="B29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="15"/>
-    </row>
-    <row r="30" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A30" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C30" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A31" s="12"/>
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="18"/>
-    </row>
-    <row r="32" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A32" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="13"/>
-    </row>
-    <row r="33" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C32" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A33" s="20"/>
       <c r="B33" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="1:3" ht="38.4" x14ac:dyDescent="0.4">
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" spans="1:4" ht="38.4" x14ac:dyDescent="0.4">
       <c r="A34" s="12" t="s">
         <v>21</v>
       </c>
@@ -1127,25 +1167,30 @@
       <c r="C34" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D34" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="19"/>
       <c r="B35" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="D35" s="21"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:4" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="10"/>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -1153,137 +1198,168 @@
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A39" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C39" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A40" s="11"/>
       <c r="B40" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="14"/>
-    </row>
-    <row r="41" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A41" s="11"/>
       <c r="B41" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="15"/>
-    </row>
-    <row r="42" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A42" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="16"/>
-    </row>
-    <row r="43" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C42" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A43" s="12"/>
       <c r="B43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="17"/>
-    </row>
-    <row r="44" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D43" s="17"/>
+    </row>
+    <row r="44" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A44" s="12"/>
       <c r="B44" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C44" s="18"/>
-    </row>
-    <row r="45" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D44" s="18"/>
+    </row>
+    <row r="45" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A45" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="13"/>
-    </row>
-    <row r="46" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C45" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="46" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A46" s="11"/>
       <c r="B46" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D46" s="14"/>
+    </row>
+    <row r="47" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A47" s="11"/>
       <c r="B47" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="15"/>
-    </row>
-    <row r="48" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D47" s="15"/>
+    </row>
+    <row r="48" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A48" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="16"/>
-    </row>
-    <row r="49" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C48" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="16"/>
+    </row>
+    <row r="49" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A49" s="12"/>
       <c r="B49" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="18"/>
-    </row>
-    <row r="50" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D49" s="18"/>
+    </row>
+    <row r="50" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A50" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="13"/>
-    </row>
-    <row r="51" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C50" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A51" s="20"/>
       <c r="B51" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="15"/>
-    </row>
-    <row r="52" spans="1:3" ht="38.4" x14ac:dyDescent="0.4">
+      <c r="D51" s="15"/>
+    </row>
+    <row r="52" spans="1:4" ht="38.4" x14ac:dyDescent="0.4">
       <c r="A52" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="16"/>
-    </row>
-    <row r="53" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C52" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="16"/>
+    </row>
+    <row r="53" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" s="19"/>
       <c r="B53" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="21"/>
-    </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="D53" s="21"/>
+    </row>
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:4" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="10"/>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D55" s="10"/>
+    </row>
+    <row r="56" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
@@ -1291,128 +1367,176 @@
         <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+        <v>42</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A57" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="13"/>
-    </row>
-    <row r="58" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C57" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="13"/>
+    </row>
+    <row r="58" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A58" s="11"/>
       <c r="B58" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="14"/>
-    </row>
-    <row r="59" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D58" s="14"/>
+    </row>
+    <row r="59" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A59" s="11"/>
       <c r="B59" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="15"/>
-    </row>
-    <row r="60" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D59" s="15"/>
+    </row>
+    <row r="60" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A60" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="16"/>
-    </row>
-    <row r="61" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C60" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="16"/>
+    </row>
+    <row r="61" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A61" s="12"/>
       <c r="B61" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="17"/>
-    </row>
-    <row r="62" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D61" s="17"/>
+    </row>
+    <row r="62" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A62" s="12"/>
       <c r="B62" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="18"/>
-    </row>
-    <row r="63" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D62" s="18"/>
+    </row>
+    <row r="63" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A63" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C63" s="13"/>
-    </row>
-    <row r="64" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C63" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" s="13"/>
+    </row>
+    <row r="64" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A64" s="11"/>
       <c r="B64" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="14"/>
-    </row>
-    <row r="65" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D64" s="14"/>
+    </row>
+    <row r="65" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A65" s="11"/>
       <c r="B65" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C65" s="15"/>
-    </row>
-    <row r="66" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D65" s="15"/>
+    </row>
+    <row r="66" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A66" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C66" s="16"/>
-    </row>
-    <row r="67" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C66" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="16"/>
+    </row>
+    <row r="67" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A67" s="12"/>
       <c r="B67" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C67" s="18"/>
-    </row>
-    <row r="68" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="D67" s="18"/>
+    </row>
+    <row r="68" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A68" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C68" s="13"/>
-    </row>
-    <row r="69" spans="1:3" ht="19.2" x14ac:dyDescent="0.4">
+      <c r="C68" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="1:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A69" s="20"/>
       <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C69" s="15"/>
-    </row>
-    <row r="70" spans="1:3" ht="38.4" x14ac:dyDescent="0.4">
+      <c r="D69" s="15"/>
+    </row>
+    <row r="70" spans="1:4" ht="38.4" x14ac:dyDescent="0.4">
       <c r="A70" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C70" s="16"/>
-    </row>
-    <row r="71" spans="1:3" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C70" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="16"/>
+    </row>
+    <row r="71" spans="1:4" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A71" s="19"/>
       <c r="B71" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="73">
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="C37:D37"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="C57:C59"/>
     <mergeCell ref="A60:A62"/>
@@ -1452,6 +1576,9 @@
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D24:D26"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C9:C11"/>

</xml_diff>